<commit_message>
Planilha de organização de testes de cards
</commit_message>
<xml_diff>
--- a/Cards para testar - Modelo.xlsx
+++ b/Cards para testar - Modelo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Testes - QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Documentos\Estudos\Cursos\Autodidata\Testes - QA\Modelos documentação de testes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DF4AD6-AC0D-44DC-8EF6-8723C6CF4945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7FBD8A-1651-49D3-9854-39AA968E7640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sprint xx" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint xx'!$A$2:$L$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint xx'!$A$2:$K$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Card (#)</t>
   </si>
@@ -93,15 +93,9 @@
     <t>Documentação de evidências</t>
   </si>
   <si>
-    <t>Validação Técnica</t>
-  </si>
-  <si>
     <t>[Especificar: Testar, Testando, Testado]</t>
   </si>
   <si>
-    <t>[Especificar: SIM ou NÃO]</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -142,12 +136,6 @@
   </si>
   <si>
     <t>TESTAR</t>
-  </si>
-  <si>
-    <t>SIM</t>
-  </si>
-  <si>
-    <t>NÃO</t>
   </si>
   <si>
     <t>Carlos</t>
@@ -270,20 +258,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -578,10 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,27 +583,26 @@
     <col min="5" max="6" width="32.44140625" style="2" customWidth="1"/>
     <col min="7" max="8" width="27.109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="20.33203125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="20.44140625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="10" max="11" width="20.44140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:11" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="2" spans="1:12" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:11" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -646,163 +636,148 @@
       <c r="K2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="J5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="8" t="s">
+      <c r="F6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -814,9 +789,8 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -828,9 +802,8 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-    </row>
-    <row r="9" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -842,9 +815,8 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-    </row>
-    <row r="10" spans="1:12" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -856,13 +828,13 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:L2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A2:K2" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="45" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>